<commit_message>
all tables added to database
</commit_message>
<xml_diff>
--- a/Data/Data-Dictionary.xlsx
+++ b/Data/Data-Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f8aab243d6baed32/Desktop/Lighthouse/After/SQL-book-learning/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="418" documentId="8_{41C11349-A933-4DD6-8D9F-0D4F65854483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F1B4F43-ACB2-4ACB-8BC5-06351308358B}"/>
+  <xr:revisionPtr revIDLastSave="446" documentId="8_{41C11349-A933-4DD6-8D9F-0D4F65854483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{626EF8C0-DEFB-4C45-8AD4-EA83BBF4C115}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{F6FB3EC1-7ABA-44D1-BCF7-427129F76C3D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="194">
   <si>
     <t>Actor Table</t>
   </si>
@@ -317,18 +317,12 @@
     <t xml:space="preserve"> language_id </t>
   </si>
   <si>
-    <t xml:space="preserve"> original_language_id </t>
-  </si>
-  <si>
     <t xml:space="preserve"> rental_duration </t>
   </si>
   <si>
     <t xml:space="preserve"> rental_rate </t>
   </si>
   <si>
-    <t xml:space="preserve"> length </t>
-  </si>
-  <si>
     <t xml:space="preserve"> replacement_cost </t>
   </si>
   <si>
@@ -359,9 +353,6 @@
     <t>A foreign key pointing at the language table; identifies the language of the film.</t>
   </si>
   <si>
-    <t>A foreign key pointing at the language table; identifies the original language of the film. Used when a film has been dubbed into a new language.</t>
-  </si>
-  <si>
     <t>The length of the rental period, in days.</t>
   </si>
   <si>
@@ -606,6 +597,27 @@
   </si>
   <si>
     <t> A foreign key identifying the address of this store.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> film_length </t>
+  </si>
+  <si>
+    <t>Film_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FID  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> price </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> actors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">film_length </t>
+  </si>
+  <si>
+    <t>The title of the movie</t>
   </si>
 </sst>
 </file>
@@ -683,6 +695,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1002,11 +1018,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6882C195-A640-4A72-8C35-451A2F3676DA}">
-  <dimension ref="A1:C155"/>
+  <dimension ref="A1:C164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1547,7 +1563,7 @@
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1558,7 +1574,7 @@
         <v>76</v>
       </c>
       <c r="C63" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1569,7 +1585,7 @@
         <v>20</v>
       </c>
       <c r="C64" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1580,7 +1596,7 @@
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1591,7 +1607,7 @@
         <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1599,10 +1615,10 @@
         <v>93</v>
       </c>
       <c r="B67" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1610,139 +1626,153 @@
         <v>94</v>
       </c>
       <c r="B68" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="C68" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>95</v>
+        <v>187</v>
       </c>
       <c r="B69" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B70" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="C70" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B71" t="s">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="C71" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B72" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="C72" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="B73" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C73" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>29</v>
-      </c>
-      <c r="B74" t="s">
-        <v>14</v>
-      </c>
-      <c r="C74" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
-        <v>100</v>
+      <c r="A76" t="s">
+        <v>189</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="B77" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C77" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="B78" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>29</v>
+        <v>145</v>
       </c>
       <c r="B79" t="s">
-        <v>14</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>190</v>
+      </c>
+      <c r="B80" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>101</v>
+      <c r="A81" t="s">
+        <v>192</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B82" t="s">
-        <v>8</v>
+        <v>77</v>
+      </c>
+      <c r="C82" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>41</v>
+        <v>191</v>
       </c>
       <c r="B83" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>29</v>
-      </c>
-      <c r="B84" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
-        <v>114</v>
+      <c r="A86" t="s">
+        <v>15</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -1752,188 +1782,156 @@
       <c r="B87" t="s">
         <v>8</v>
       </c>
-      <c r="C87" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="B88" t="s">
-        <v>76</v>
-      </c>
-      <c r="C88" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>115</v>
-      </c>
-      <c r="B89" t="s">
-        <v>20</v>
-      </c>
-      <c r="C89" t="s">
-        <v>104</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
-        <v>116</v>
+      <c r="A91" t="s">
+        <v>88</v>
+      </c>
+      <c r="B91" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="B92" t="s">
         <v>8</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
+        <v>29</v>
+      </c>
+      <c r="B93" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>88</v>
       </c>
-      <c r="B93" t="s">
-        <v>8</v>
-      </c>
-      <c r="C93" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>59</v>
-      </c>
-      <c r="B94" t="s">
-        <v>8</v>
-      </c>
-      <c r="C94" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>29</v>
-      </c>
-      <c r="B95" t="s">
-        <v>14</v>
-      </c>
-      <c r="C95" t="s">
-        <v>13</v>
+      <c r="B96" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
-        <v>121</v>
+      <c r="A97" t="s">
+        <v>89</v>
+      </c>
+      <c r="B97" t="s">
+        <v>76</v>
+      </c>
+      <c r="C97" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="B98" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C98" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>122</v>
-      </c>
-      <c r="B99" t="s">
-        <v>77</v>
-      </c>
-      <c r="C99" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>29</v>
-      </c>
-      <c r="B100" t="s">
-        <v>14</v>
-      </c>
-      <c r="C100" t="s">
-        <v>13</v>
+      <c r="A100" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>114</v>
+      </c>
+      <c r="B101" t="s">
+        <v>8</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
-        <v>125</v>
+      <c r="A102" t="s">
+        <v>88</v>
+      </c>
+      <c r="B102" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>126</v>
+        <v>59</v>
       </c>
       <c r="B103" t="s">
         <v>8</v>
       </c>
       <c r="C103" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="B104" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C104" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>127</v>
-      </c>
-      <c r="B105" t="s">
-        <v>8</v>
-      </c>
-      <c r="C105" t="s">
-        <v>134</v>
+        <v>13</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>128</v>
-      </c>
-      <c r="B106" t="s">
-        <v>8</v>
-      </c>
-      <c r="C106" t="s">
-        <v>135</v>
+      <c r="A106" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="B107" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="C107" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B108" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="C108" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
@@ -1949,62 +1947,62 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B112" t="s">
         <v>8</v>
       </c>
       <c r="C112" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>139</v>
+        <v>58</v>
       </c>
       <c r="B113" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C113" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B114" t="s">
         <v>8</v>
       </c>
       <c r="C114" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="B115" t="s">
         <v>8</v>
       </c>
       <c r="C115" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B116" t="s">
-        <v>14</v>
+        <v>128</v>
       </c>
       <c r="C116" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -2012,10 +2010,10 @@
         <v>127</v>
       </c>
       <c r="B117" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C117" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -2031,192 +2029,192 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="B121" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C121" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B122" t="s">
-        <v>131</v>
+        <v>14</v>
       </c>
       <c r="C122" t="s">
-        <v>151</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>114</v>
+      </c>
+      <c r="B123" t="s">
+        <v>8</v>
+      </c>
+      <c r="C123" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
-        <v>152</v>
+      <c r="A124" t="s">
+        <v>58</v>
+      </c>
+      <c r="B124" t="s">
+        <v>8</v>
+      </c>
+      <c r="C124" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="B125" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C125" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C126" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>149</v>
+        <v>29</v>
       </c>
       <c r="B127" t="s">
-        <v>131</v>
+        <v>14</v>
       </c>
       <c r="C127" t="s">
-        <v>157</v>
+        <v>13</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="B130" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="C130" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B131" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="C131" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>160</v>
-      </c>
-      <c r="B132" t="s">
-        <v>77</v>
-      </c>
-      <c r="C132" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>22</v>
-      </c>
-      <c r="B133" t="s">
-        <v>8</v>
-      </c>
-      <c r="C133" t="s">
-        <v>165</v>
+      <c r="A133" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="B134" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C134" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="B135" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="C135" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>61</v>
+        <v>146</v>
       </c>
       <c r="B136" t="s">
-        <v>63</v>
+        <v>128</v>
       </c>
       <c r="C136" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>161</v>
-      </c>
-      <c r="B137" t="s">
-        <v>77</v>
-      </c>
-      <c r="C137" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
-        <v>171</v>
-      </c>
-      <c r="B138" t="s">
-        <v>31</v>
-      </c>
-      <c r="C138" t="s">
-        <v>170</v>
+      <c r="A138" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="B139" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C139" t="s">
-        <v>13</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>156</v>
+      </c>
+      <c r="B140" t="s">
+        <v>77</v>
+      </c>
+      <c r="C140" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" s="1" t="s">
-        <v>172</v>
+      <c r="A141" t="s">
+        <v>157</v>
+      </c>
+      <c r="B141" t="s">
+        <v>77</v>
+      </c>
+      <c r="C141" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>173</v>
+        <v>22</v>
       </c>
       <c r="B142" t="s">
         <v>8</v>
@@ -2227,124 +2225,206 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>184</v>
+        <v>60</v>
       </c>
       <c r="B143" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C143" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>174</v>
+        <v>59</v>
       </c>
       <c r="B144" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C144" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="B145" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="C145" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="B146" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="C146" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B147" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C147" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>177</v>
+        <v>29</v>
       </c>
       <c r="B148" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C148" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>75</v>
-      </c>
-      <c r="B149" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151" s="1" t="s">
-        <v>185</v>
+      <c r="A151" t="s">
+        <v>170</v>
+      </c>
+      <c r="B151" t="s">
+        <v>8</v>
+      </c>
+      <c r="C151" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>59</v>
+        <v>181</v>
       </c>
       <c r="B152" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C152" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="B153" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C153" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="B154" t="s">
         <v>8</v>
       </c>
       <c r="C154" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
+        <v>172</v>
+      </c>
+      <c r="B155" t="s">
+        <v>8</v>
+      </c>
+      <c r="C155" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>173</v>
+      </c>
+      <c r="B156" t="s">
+        <v>42</v>
+      </c>
+      <c r="C156" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>174</v>
+      </c>
+      <c r="B157" t="s">
+        <v>42</v>
+      </c>
+      <c r="C157" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>75</v>
+      </c>
+      <c r="B158" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>59</v>
+      </c>
+      <c r="B161" t="s">
+        <v>8</v>
+      </c>
+      <c r="C161" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>183</v>
+      </c>
+      <c r="B162" t="s">
+        <v>8</v>
+      </c>
+      <c r="C162" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>22</v>
+      </c>
+      <c r="B163" t="s">
+        <v>8</v>
+      </c>
+      <c r="C163" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
         <v>29</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B164" t="s">
         <v>14</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C164" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>